<commit_message>
All tables for indices in
</commit_message>
<xml_diff>
--- a/txt_files/Fleet10and11_MRFSSDockside_IndexData.xlsx
+++ b/txt_files/Fleet10and11_MRFSSDockside_IndexData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="4485" tabRatio="789" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NorthAIC" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>Model</t>
   </si>
@@ -86,21 +86,12 @@
     <t>Year + Region</t>
   </si>
   <si>
-    <t>Year + Region + Area_X</t>
-  </si>
-  <si>
     <t>AIC</t>
   </si>
   <si>
     <t>Year+ Wave</t>
   </si>
   <si>
-    <t>Year + Wave + Area_X</t>
-  </si>
-  <si>
-    <t>Year + Wave + Area_X + SubRegion</t>
-  </si>
-  <si>
     <t>Year + Wave + SubRegion</t>
   </si>
   <si>
@@ -110,7 +101,49 @@
     <t>\textbf{537}</t>
   </si>
   <si>
-    <t>Year + Region + Area_X + Wave</t>
+    <t>1,481</t>
+  </si>
+  <si>
+    <t>1,429</t>
+  </si>
+  <si>
+    <t>1,403</t>
+  </si>
+  <si>
+    <t>1,397</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Year + Region + Area\_X</t>
+  </si>
+  <si>
+    <t>Year + Region + Area\_X + Wave</t>
+  </si>
+  <si>
+    <t>Year + Wave + Area\_X</t>
+  </si>
+  <si>
+    <t>Year + Wave + Area\_X + SubRegion</t>
+  </si>
+  <si>
+    <t>10,392</t>
+  </si>
+  <si>
+    <t>10,327</t>
+  </si>
+  <si>
+    <t>10,122</t>
+  </si>
+  <si>
+    <t>2,788</t>
+  </si>
+  <si>
+    <t>7,334</t>
+  </si>
+  <si>
+    <t>1,061</t>
   </si>
 </sst>
 </file>
@@ -193,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -209,6 +242,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,49 +526,52 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="28.3828125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>1481</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3">
-        <v>1429</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B5">
-        <v>1397</v>
       </c>
     </row>
   </sheetData>
@@ -547,12 +584,15 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="53.15234375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -574,9 +614,9 @@
         <v>552</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>908</v>
@@ -585,9 +625,9 @@
         <v>538</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>905</v>
@@ -596,20 +636,20 @@
         <v>540</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>908</v>
@@ -625,15 +665,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -644,66 +684,148 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>10392</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
-        <v>10327</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2">
-        <v>10122</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="7">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="7">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7">
+        <v>806</v>
+      </c>
+      <c r="C8" s="7">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7">
+        <v>623</v>
+      </c>
+      <c r="C9" s="7">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="7">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7">
+        <v>687</v>
+      </c>
+      <c r="C13" s="7">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="7">
+        <v>430</v>
+      </c>
+      <c r="C14" s="7">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -715,12 +837,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -731,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -742,7 +864,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -753,7 +875,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -764,7 +886,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -785,12 +907,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -801,7 +923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -812,7 +934,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -823,7 +945,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -834,7 +956,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -858,9 +980,9 @@
       <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -871,7 +993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>1984</v>
       </c>
@@ -882,7 +1004,7 @@
         <v>0.60399999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>1985</v>
       </c>
@@ -893,7 +1015,7 @@
         <v>0.54844999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>1986</v>
       </c>
@@ -904,7 +1026,7 @@
         <v>0.57948</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>1987</v>
       </c>
@@ -915,7 +1037,7 @@
         <v>0.66464999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>1988</v>
       </c>
@@ -926,7 +1048,7 @@
         <v>0.61219999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>1989</v>
       </c>
@@ -937,7 +1059,7 @@
         <v>0.66225999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>1995</v>
       </c>
@@ -948,7 +1070,7 @@
         <v>0.64163000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>1996</v>
       </c>
@@ -959,7 +1081,7 @@
         <v>0.52497000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>1999</v>
       </c>
@@ -970,31 +1092,31 @@
         <v>0.53354000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
     </row>
   </sheetData>
@@ -1007,13 +1129,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1024,7 +1146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1980</v>
       </c>
@@ -1035,7 +1157,7 @@
         <v>0.212394</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>1981</v>
       </c>
@@ -1046,7 +1168,7 @@
         <v>0.24019099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>1982</v>
       </c>
@@ -1057,7 +1179,7 @@
         <v>0.248533</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>1983</v>
       </c>
@@ -1068,7 +1190,7 @@
         <v>0.12693499999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>1984</v>
       </c>
@@ -1079,7 +1201,7 @@
         <v>0.16721</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>1985</v>
       </c>
@@ -1090,7 +1212,7 @@
         <v>0.209593</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>1986</v>
       </c>
@@ -1101,7 +1223,7 @@
         <v>0.185109</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>1996</v>
       </c>
@@ -1112,7 +1234,7 @@
         <v>0.27595199999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>1998</v>
       </c>
@@ -1123,7 +1245,7 @@
         <v>0.258855</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>1999</v>
       </c>

</xml_diff>

<commit_message>
Drafted fishery-dependent indices except length comps
</commit_message>
<xml_diff>
--- a/txt_files/Fleet10and11_MRFSSDockside_IndexData.xlsx
+++ b/txt_files/Fleet10and11_MRFSSDockside_IndexData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="4485" tabRatio="789" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NorthAIC" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>Model</t>
   </si>
@@ -144,6 +144,21 @@
   </si>
   <si>
     <t>1,061</t>
+  </si>
+  <si>
+    <t>Remove years after 1999 due to regulation changes and with fewer than 20 trips</t>
+  </si>
+  <si>
+    <t>544</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>Stephens-MacCall filter (keep all positives - selected filter)</t>
+  </si>
+  <si>
+    <t>Alternate Stephens-MacCall filter (keep only above threshold)</t>
   </si>
 </sst>
 </file>
@@ -529,12 +544,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.3828125" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -550,7 +565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -558,7 +573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -566,7 +581,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -587,12 +602,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.15234375" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -614,7 +629,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -625,7 +640,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -636,7 +651,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -647,7 +662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -665,15 +680,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="65.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -684,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -695,7 +713,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -706,7 +724,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -717,7 +735,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -728,7 +746,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -739,7 +757,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -750,9 +768,9 @@
         <v>620</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B8" s="7">
         <v>806</v>
@@ -761,9 +779,9 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B9" s="7">
         <v>623</v>
@@ -772,31 +790,31 @@
         <v>437</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="7">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>36</v>
@@ -805,26 +823,48 @@
         <v>441</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="7">
-        <v>687</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="C13" s="7">
         <v>441</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B14" s="7">
+        <v>687</v>
+      </c>
+      <c r="C14" s="7">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="7">
         <v>430</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C15" s="7">
         <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <v>475</v>
+      </c>
+      <c r="C16" s="7">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -840,9 +880,9 @@
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -853,7 +893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -864,7 +904,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -875,7 +915,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -886,7 +926,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -910,9 +950,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -923,7 +963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -934,7 +974,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -945,7 +985,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -956,7 +996,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -980,9 +1020,9 @@
       <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -993,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1984</v>
       </c>
@@ -1004,7 +1044,7 @@
         <v>0.60399999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1985</v>
       </c>
@@ -1015,7 +1055,7 @@
         <v>0.54844999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1986</v>
       </c>
@@ -1026,7 +1066,7 @@
         <v>0.57948</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1987</v>
       </c>
@@ -1037,7 +1077,7 @@
         <v>0.66464999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>1988</v>
       </c>
@@ -1048,7 +1088,7 @@
         <v>0.61219999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>1989</v>
       </c>
@@ -1059,7 +1099,7 @@
         <v>0.66225999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>1995</v>
       </c>
@@ -1070,7 +1110,7 @@
         <v>0.64163000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1996</v>
       </c>
@@ -1081,7 +1121,7 @@
         <v>0.52497000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>1999</v>
       </c>
@@ -1092,31 +1132,31 @@
         <v>0.53354000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
     </row>
   </sheetData>
@@ -1133,9 +1173,9 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1146,7 +1186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1980</v>
       </c>
@@ -1157,7 +1197,7 @@
         <v>0.212394</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1981</v>
       </c>
@@ -1168,7 +1208,7 @@
         <v>0.24019099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1982</v>
       </c>
@@ -1179,7 +1219,7 @@
         <v>0.248533</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1983</v>
       </c>
@@ -1190,7 +1230,7 @@
         <v>0.12693499999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1984</v>
       </c>
@@ -1201,7 +1241,7 @@
         <v>0.16721</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1985</v>
       </c>
@@ -1212,7 +1252,7 @@
         <v>0.209593</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>1986</v>
       </c>
@@ -1223,7 +1263,7 @@
         <v>0.185109</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1996</v>
       </c>
@@ -1234,7 +1274,7 @@
         <v>0.27595199999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1998</v>
       </c>
@@ -1245,7 +1285,7 @@
         <v>0.258855</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>1999</v>
       </c>

</xml_diff>

<commit_message>
Added final edits from John. Copy sent to Devo, Stacey, John F, and Owen
</commit_message>
<xml_diff>
--- a/txt_files/Fleet10and11_MRFSSDockside_IndexData.xlsx
+++ b/txt_files/Fleet10and11_MRFSSDockside_IndexData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="4485" tabRatio="789" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789"/>
   </bookViews>
   <sheets>
     <sheet name="NorthAIC" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>1,403</t>
   </si>
   <si>
-    <t>1,397</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Alternate Stephens-MacCall filter (keep only above threshold)</t>
+  </si>
+  <si>
+    <t>\textbf{1,397}</t>
   </si>
 </sst>
 </file>
@@ -540,16 +540,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -565,7 +565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -573,20 +573,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -602,12 +602,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="1" max="1" width="53.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -629,7 +629,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -640,9 +640,9 @@
         <v>538</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>905</v>
@@ -651,9 +651,9 @@
         <v>540</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -662,7 +662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -682,16 +682,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -702,75 +702,75 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="7">
         <v>620</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="7">
         <v>620</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="7">
         <v>806</v>
@@ -779,9 +779,9 @@
         <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="7">
         <v>623</v>
@@ -790,53 +790,53 @@
         <v>437</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7">
         <v>441</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
         <v>441</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="7">
         <v>687</v>
@@ -845,9 +845,9 @@
         <v>441</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="7">
         <v>430</v>
@@ -856,9 +856,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>475</v>
@@ -880,9 +880,9 @@
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -893,7 +893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -904,7 +904,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -915,7 +915,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -926,7 +926,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -950,9 +950,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -963,7 +963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -974,7 +974,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -985,7 +985,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -996,7 +996,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1020,9 +1020,9 @@
       <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>1984</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>0.60399999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>1985</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>0.54844999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>1986</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>0.57948</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>1987</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>0.66464999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>1988</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>0.61219999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>1989</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>0.66225999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>1995</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>0.64163000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>1996</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>0.52497000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>1999</v>
       </c>
@@ -1132,31 +1132,31 @@
         <v>0.53354000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
     </row>
   </sheetData>
@@ -1173,9 +1173,9 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1980</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>0.212394</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>1981</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>0.24019099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>1982</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>0.248533</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>1983</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>0.12693499999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>1984</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>0.16721</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>1985</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>0.209593</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>1986</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>0.185109</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>1996</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>0.27595199999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>1998</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>0.258855</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>1999</v>
       </c>

</xml_diff>

<commit_message>
Added in comments received
</commit_message>
<xml_diff>
--- a/txt_files/Fleet10and11_MRFSSDockside_IndexData.xlsx
+++ b/txt_files/Fleet10and11_MRFSSDockside_IndexData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NorthAIC" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>Model</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Remove north of Cape Mendocino</t>
   </si>
   <si>
-    <t>Remove trips targetting offshore species</t>
-  </si>
-  <si>
     <t>Remove species that never co-occurand  not present in at least 1% of all</t>
   </si>
   <si>
@@ -159,6 +156,12 @@
   </si>
   <si>
     <t>\textbf{1,397}</t>
+  </si>
+  <si>
+    <t>Remove trips targeting offshore species</t>
+  </si>
+  <si>
+    <t>Remove species that never co-occur and  not present in at least 1% of all</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -554,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -562,31 +565,31 @@
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +634,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>908</v>
@@ -642,7 +645,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>905</v>
@@ -653,18 +656,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>908</v>
@@ -682,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -707,10 +710,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -718,40 +721,40 @@
         <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="7">
         <v>620</v>
@@ -759,10 +762,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="7">
         <v>620</v>
@@ -770,7 +773,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="7">
         <v>806</v>
@@ -781,7 +784,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="7">
         <v>623</v>
@@ -792,32 +795,32 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7">
         <v>441</v>
@@ -825,10 +828,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="7">
         <v>441</v>
@@ -836,7 +839,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="7">
         <v>687</v>
@@ -847,7 +850,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7">
         <v>430</v>
@@ -858,7 +861,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>475</v>
@@ -895,7 +898,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>2788</v>
@@ -906,7 +909,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <v>2788</v>
@@ -917,7 +920,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>806</v>
@@ -928,7 +931,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>623</v>
@@ -965,7 +968,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>7334</v>
@@ -976,7 +979,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <v>7334</v>
@@ -987,7 +990,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2">
         <v>687</v>
@@ -998,7 +1001,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <v>430</v>

</xml_diff>